<commit_message>
L2 : jUnit corectat
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB15CF05-54B5-469D-8F39-9831DAEEB8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFDDB7B-A04B-47AF-BA10-33F60A17064D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="125">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -170,6 +170,372 @@
   </si>
   <si>
     <t>Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
+  </si>
+  <si>
+    <t>Observații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
+  </si>
+  <si>
+    <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
+  </si>
+  <si>
+    <t>3. Se aleg doi parametri ai metodei testate şi se definesc condiţii asupra acestora. Condiţiile (constrângerile) rezultă din specificaţii.</t>
+  </si>
+  <si>
+    <t>4. Pentru aceşti parametri se aplică ECP şi BVA. La proiectarea testelor se consideră că parametrii de intrare neinvestigaţi aici au valori valide, adică folosim dummy objects.</t>
+  </si>
+  <si>
+    <t>EC Identification</t>
+  </si>
+  <si>
+    <t>EC-based TCs</t>
+  </si>
+  <si>
+    <t>No. EC</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Valid EC</t>
+  </si>
+  <si>
+    <t>Non-valid EC</t>
+  </si>
+  <si>
+    <t>No. TCxx_EC</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>input data</t>
+  </si>
+  <si>
+    <t>output data</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>2,3,2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BVA Condition</t>
+  </si>
+  <si>
+    <t>BVA Condition-based TCs</t>
+  </si>
+  <si>
+    <t>Crt. No.</t>
+  </si>
+  <si>
+    <t>No TCxx_BVA</t>
+  </si>
+  <si>
+    <t>BVA condition</t>
+  </si>
+  <si>
+    <t>Correlated TC</t>
+  </si>
+  <si>
+    <t>Executable</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>BBT TCs</t>
+  </si>
+  <si>
+    <t>Final        TC No.</t>
+  </si>
+  <si>
+    <t>Req. ID</t>
+  </si>
+  <si>
+    <t>ECP TCs</t>
+  </si>
+  <si>
+    <t>BVA TCs</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>TC1_ECP</t>
+  </si>
+  <si>
+    <t>TC3_ECP</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Re-testing</t>
+  </si>
+  <si>
+    <t>Regression Testing</t>
+  </si>
+  <si>
+    <t>#TCs to be run</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="17"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>passed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#TCs    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>failed</t>
+    </r>
+  </si>
+  <si>
+    <t>#Bugs</t>
+  </si>
+  <si>
+    <t>#Fixed Bugs</t>
+  </si>
+  <si>
+    <t>Re-tested</t>
+  </si>
+  <si>
+    <t>Varga Gabriela</t>
+  </si>
+  <si>
+    <t>Voina Marius</t>
+  </si>
+  <si>
+    <t>addProduct(String name, double price, int inStock, int min, int  max, ObservableList&lt;Part&gt; addParts)</t>
+  </si>
+  <si>
+    <t>max este mai mare sau egal dacet min</t>
+  </si>
+  <si>
+    <t>inStock este mai mare sau egal decat min</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 7</t>
+  </si>
+  <si>
+    <t>nume</t>
+  </si>
+  <si>
+    <t>pret</t>
+  </si>
+  <si>
+    <t>inStock</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>addParts</t>
+  </si>
+  <si>
+    <t>produs adaugat</t>
+  </si>
+  <si>
+    <t>2, 3, 5, 7</t>
+  </si>
+  <si>
+    <t>"ghinion"</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 8</t>
+  </si>
+  <si>
+    <t>cioburi de oglinda</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>1, 3, 6, 7</t>
+  </si>
+  <si>
+    <t>"fericire"</t>
+  </si>
+  <si>
+    <t>bani, prieteni</t>
+  </si>
+  <si>
+    <t>Error message-</t>
+  </si>
+  <si>
+    <t>"rabdare"</t>
+  </si>
+  <si>
+    <t>"IQ"</t>
+  </si>
+  <si>
+    <t>fericire, timp liber</t>
+  </si>
+  <si>
+    <t>01. min = -1</t>
+  </si>
+  <si>
+    <t>02. min = 0</t>
+  </si>
+  <si>
+    <t>03. min = 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parametrii </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="30"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>min, max si inStack; Condiţii pentru aceşti parametri de intrare: min, max si inStock sunt valide daca min &lt;= inStock &lt;= max, unde min, max reale pozitive, iar inStock natural.</t>
+    </r>
+  </si>
+  <si>
+    <t>min este pozitiv</t>
+  </si>
+  <si>
+    <t>min nu e pozitiv</t>
+  </si>
+  <si>
+    <t>pretul este pozitiv</t>
+  </si>
+  <si>
+    <t>pretul nu este pozitiv</t>
+  </si>
+  <si>
+    <t>min este pozitiv si &lt;= INT_MAX - 1</t>
+  </si>
+  <si>
+    <t>04. min = INT_MAX - 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05. min = INT_MAX </t>
+  </si>
+  <si>
+    <t>06. min = INT_MAX + 1</t>
+  </si>
+  <si>
+    <t>min &lt;= max</t>
+  </si>
+  <si>
+    <t>08. min = max</t>
+  </si>
+  <si>
+    <t>07. min = max - 1</t>
+  </si>
+  <si>
+    <t>09. min = max + 1</t>
+  </si>
+  <si>
+    <t>creier</t>
+  </si>
+  <si>
+    <t>max &gt;= min</t>
+  </si>
+  <si>
+    <t>max &lt; min</t>
+  </si>
+  <si>
+    <t>inStock &gt;= min</t>
+  </si>
+  <si>
+    <t>inStock &lt; min</t>
+  </si>
+  <si>
+    <t>10. inStock = min-1</t>
+  </si>
+  <si>
+    <t>11. inStock = min</t>
+  </si>
+  <si>
+    <t>12. inStock = min + 1</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC4_ECP</t>
+  </si>
+  <si>
+    <t>TC1_BVA</t>
+  </si>
+  <si>
+    <t>TC2_BVA</t>
+  </si>
+  <si>
+    <t>TC8_BVA</t>
+  </si>
+  <si>
+    <t>TC10_BVA</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>familie</t>
+  </si>
+  <si>
+    <t>pisica neagra</t>
+  </si>
+  <si>
+    <t>Nu exista metoda equals pentru parts sau products</t>
+  </si>
+  <si>
+    <t>Implementarea metodelor</t>
+  </si>
+  <si>
+    <t>Nu se valideaza datele pe backend</t>
+  </si>
+  <si>
+    <t>Adaugarea codului de validare datelor in metoda</t>
+  </si>
+  <si>
+    <t>Prinderea exceptiilor de la validare din service in UI</t>
+  </si>
+  <si>
+    <t>Adaugrea codului</t>
   </si>
   <si>
     <r>
@@ -190,386 +556,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> adăugarea unui film nou (titlu, regizor, an aparitie, actori, categorie, cuvinte cheie);</t>
+      <t xml:space="preserve"> addProduct(String name, double price, int inStock, int min, int  max, ObservableList&lt;Part&gt; addParts)</t>
     </r>
-  </si>
-  <si>
-    <t>Observații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
-  </si>
-  <si>
-    <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
-  </si>
-  <si>
-    <t>3. Se aleg doi parametri ai metodei testate şi se definesc condiţii asupra acestora. Condiţiile (constrângerile) rezultă din specificaţii.</t>
-  </si>
-  <si>
-    <t>4. Pentru aceşti parametri se aplică ECP şi BVA. La proiectarea testelor se consideră că parametrii de intrare neinvestigaţi aici au valori valide, adică folosim dummy objects.</t>
-  </si>
-  <si>
-    <t>EC Identification</t>
-  </si>
-  <si>
-    <t>EC-based TCs</t>
-  </si>
-  <si>
-    <t>No. EC</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Valid EC</t>
-  </si>
-  <si>
-    <t>Non-valid EC</t>
-  </si>
-  <si>
-    <t>No. TCxx_EC</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>input data</t>
-  </si>
-  <si>
-    <t>output data</t>
-  </si>
-  <si>
-    <t>expected</t>
-  </si>
-  <si>
-    <t>2,3,2</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>BVA Condition</t>
-  </si>
-  <si>
-    <t>BVA Condition-based TCs</t>
-  </si>
-  <si>
-    <t>Crt. No.</t>
-  </si>
-  <si>
-    <t>No TCxx_BVA</t>
-  </si>
-  <si>
-    <t>BVA condition</t>
-  </si>
-  <si>
-    <t>Correlated TC</t>
-  </si>
-  <si>
-    <t>Executable</t>
-  </si>
-  <si>
-    <t>expected result</t>
-  </si>
-  <si>
-    <t>BBT TCs</t>
-  </si>
-  <si>
-    <t>Final        TC No.</t>
-  </si>
-  <si>
-    <t>Req. ID</t>
-  </si>
-  <si>
-    <t>ECP TCs</t>
-  </si>
-  <si>
-    <t>BVA TCs</t>
-  </si>
-  <si>
-    <t>F01</t>
-  </si>
-  <si>
-    <t>TC1_ECP</t>
-  </si>
-  <si>
-    <t>TC3_ECP</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Debugging</t>
-  </si>
-  <si>
-    <t>Re-testing</t>
-  </si>
-  <si>
-    <t>Regression Testing</t>
-  </si>
-  <si>
-    <t>#TCs to be run</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="17"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>passed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#TCs    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>failed</t>
-    </r>
-  </si>
-  <si>
-    <t>#Bugs</t>
-  </si>
-  <si>
-    <t>#Fixed Bugs</t>
-  </si>
-  <si>
-    <t>Re-tested</t>
-  </si>
-  <si>
-    <t>Varga Gabriela</t>
-  </si>
-  <si>
-    <t>Voina Marius</t>
-  </si>
-  <si>
-    <t>addProduct(String name, double price, int inStock, int min, int  max, ObservableList&lt;Part&gt; addParts)</t>
-  </si>
-  <si>
-    <t>max este mai mare sau egal dacet min</t>
-  </si>
-  <si>
-    <t>inStock este mai mare sau egal decat min</t>
-  </si>
-  <si>
-    <t>1, 3, 5, 7</t>
-  </si>
-  <si>
-    <t>nume</t>
-  </si>
-  <si>
-    <t>pret</t>
-  </si>
-  <si>
-    <t>inStock</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>addParts</t>
-  </si>
-  <si>
-    <t>produs adaugat</t>
-  </si>
-  <si>
-    <t>2, 3, 5, 7</t>
-  </si>
-  <si>
-    <t>"ghinion"</t>
-  </si>
-  <si>
-    <t>1, 3, 5, 8</t>
-  </si>
-  <si>
-    <t>cioburi de oglinda</t>
-  </si>
-  <si>
-    <t>Error message</t>
-  </si>
-  <si>
-    <t>1, 3, 6, 7</t>
-  </si>
-  <si>
-    <t>"fericire"</t>
-  </si>
-  <si>
-    <t>bani, prieteni</t>
-  </si>
-  <si>
-    <t>Error message-</t>
-  </si>
-  <si>
-    <t>"rabdare"</t>
-  </si>
-  <si>
-    <t>"IQ"</t>
-  </si>
-  <si>
-    <t>fericire, timp liber</t>
-  </si>
-  <si>
-    <t>01. min = -1</t>
-  </si>
-  <si>
-    <t>02. min = 0</t>
-  </si>
-  <si>
-    <t>03. min = 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Parametrii </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="30"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>min, max si inStack; Condiţii pentru aceşti parametri de intrare: min, max si inStock sunt valide daca min &lt;= inStock &lt;= max, unde min, max reale pozitive, iar inStock natural.</t>
-    </r>
-  </si>
-  <si>
-    <t>min este pozitiv</t>
-  </si>
-  <si>
-    <t>min nu e pozitiv</t>
-  </si>
-  <si>
-    <t>pretul este pozitiv</t>
-  </si>
-  <si>
-    <t>pretul nu este pozitiv</t>
-  </si>
-  <si>
-    <t>min este pozitiv si &lt;= INT_MAX - 1</t>
-  </si>
-  <si>
-    <t>04. min = INT_MAX - 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05. min = INT_MAX </t>
-  </si>
-  <si>
-    <t>06. min = INT_MAX + 1</t>
-  </si>
-  <si>
-    <t>min &lt;= max</t>
-  </si>
-  <si>
-    <t>08. min = max</t>
-  </si>
-  <si>
-    <t>07. min = max - 1</t>
-  </si>
-  <si>
-    <t>09. min = max + 1</t>
-  </si>
-  <si>
-    <t>TC_02</t>
-  </si>
-  <si>
-    <t>TC_01</t>
-  </si>
-  <si>
-    <t>creier</t>
-  </si>
-  <si>
-    <t>TC_08</t>
-  </si>
-  <si>
-    <t>max &gt;= min</t>
-  </si>
-  <si>
-    <t>max &lt; min</t>
-  </si>
-  <si>
-    <t>inStock &gt;= min</t>
-  </si>
-  <si>
-    <t>inStock &lt; min</t>
-  </si>
-  <si>
-    <t>10. inStock = min-1</t>
-  </si>
-  <si>
-    <t>11. inStock = min</t>
-  </si>
-  <si>
-    <t>12. inStock = min + 1</t>
-  </si>
-  <si>
-    <t>TC_10</t>
-  </si>
-  <si>
-    <t>TC2_ECP</t>
-  </si>
-  <si>
-    <t>TC4_ECP</t>
-  </si>
-  <si>
-    <t>TC1_BVA</t>
-  </si>
-  <si>
-    <t>TC2_BVA</t>
-  </si>
-  <si>
-    <t>TC8_BVA</t>
-  </si>
-  <si>
-    <t>TC10_BVA</t>
-  </si>
-  <si>
-    <t>actual</t>
-  </si>
-  <si>
-    <t>familie</t>
-  </si>
-  <si>
-    <t>pisica neagra</t>
-  </si>
-  <si>
-    <t>Nu exista metoda equals pentru parts sau products</t>
-  </si>
-  <si>
-    <t>Implementarea metodelor</t>
-  </si>
-  <si>
-    <t>Nu se valideaza datele pe backend</t>
-  </si>
-  <si>
-    <t>Adaugarea codului de validare datelor in metoda</t>
-  </si>
-  <si>
-    <t>Prinderea exceptiilor de la validare din service in UI</t>
-  </si>
-  <si>
-    <t>Adaugrea codului</t>
   </si>
 </sst>
 </file>
@@ -1806,8 +1794,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView topLeftCell="A9" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1853,7 +1841,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J4" s="2">
         <v>237</v>
@@ -1864,7 +1852,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="2">
         <v>237</v>
@@ -1929,7 +1917,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1942,27 +1930,27 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1979,7 +1967,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1997,7 +1985,7 @@
     <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
@@ -2034,7 +2022,7 @@
   <dimension ref="B1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2067,7 +2055,7 @@
     </row>
     <row r="3" spans="2:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -2078,13 +2066,13 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
       <c r="G5" s="42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
@@ -2099,25 +2087,25 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="G6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="H6" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="I6" s="53" t="s">
         <v>27</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>28</v>
       </c>
       <c r="J6" s="54"/>
       <c r="K6" s="54"/>
@@ -2126,7 +2114,7 @@
       <c r="N6" s="54"/>
       <c r="O6" s="55"/>
       <c r="P6" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="52"/>
     </row>
@@ -2135,35 +2123,35 @@
         <v>1</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="11"/>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="53" t="s">
         <v>71</v>
-      </c>
-      <c r="N7" s="53" t="s">
-        <v>72</v>
       </c>
       <c r="O7" s="55"/>
       <c r="P7" s="53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="55"/>
     </row>
@@ -2174,16 +2162,16 @@
       <c r="C8" s="50"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" s="12">
         <v>5000</v>
@@ -2198,13 +2186,13 @@
         <v>1000000</v>
       </c>
       <c r="N8" s="45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q8" s="46"/>
     </row>
@@ -2213,20 +2201,20 @@
         <v>3</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E9" s="11"/>
       <c r="G9" s="10">
         <v>2</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" s="12">
         <v>-2000</v>
@@ -2241,13 +2229,13 @@
         <v>100</v>
       </c>
       <c r="N9" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P9" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q9" s="46"/>
     </row>
@@ -2258,16 +2246,16 @@
       <c r="C10" s="50"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G10" s="10">
         <v>3</v>
       </c>
       <c r="H10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="J10" s="12">
         <v>1000000000</v>
@@ -2282,11 +2270,11 @@
         <v>100</v>
       </c>
       <c r="N10" s="45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O10" s="46"/>
       <c r="P10" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q10" s="46"/>
     </row>
@@ -2295,20 +2283,20 @@
         <v>5</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E11" s="11"/>
       <c r="G11" s="10">
         <v>4</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" s="12">
         <v>1000000000</v>
@@ -2323,11 +2311,11 @@
         <v>100</v>
       </c>
       <c r="N11" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O11" s="46"/>
       <c r="P11" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q11" s="46"/>
     </row>
@@ -2338,7 +2326,7 @@
       <c r="C12" s="50"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="12"/>
@@ -2357,10 +2345,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="11"/>
       <c r="G13" s="10"/>
@@ -2382,7 +2370,7 @@
       <c r="C14" s="50"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="12"/>
@@ -2501,7 +2489,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D22" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="57"/>
       <c r="G22" s="57"/>
@@ -2561,8 +2549,8 @@
   </sheetPr>
   <dimension ref="B1:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="C3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2598,7 +2586,7 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" s="78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="71"/>
       <c r="D3" s="71"/>
@@ -2609,12 +2597,12 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B5" s="75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="75"/>
       <c r="D5" s="75"/>
       <c r="G5" s="72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="72"/>
       <c r="I5" s="72"/>
@@ -2630,28 +2618,28 @@
     </row>
     <row r="6" spans="2:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="61" t="s">
+      <c r="H6" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="61" t="s">
+      <c r="I6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="J6" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="63" t="s">
-        <v>40</v>
-      </c>
       <c r="K6" s="73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="79"/>
       <c r="M6" s="79"/>
@@ -2659,7 +2647,7 @@
       <c r="O6" s="79"/>
       <c r="P6" s="74"/>
       <c r="Q6" s="73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R6" s="74"/>
     </row>
@@ -2668,35 +2656,35 @@
         <v>1</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="62"/>
       <c r="H7" s="62"/>
       <c r="I7" s="62"/>
       <c r="J7" s="64"/>
       <c r="K7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="M7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="N7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="O7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="P7" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="P7" s="19" t="s">
-        <v>72</v>
-      </c>
       <c r="Q7" s="73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R7" s="74"/>
     </row>
@@ -2704,7 +2692,7 @@
       <c r="B8" s="66"/>
       <c r="C8" s="69"/>
       <c r="D8" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G8" s="19">
         <v>1</v>
@@ -2712,12 +2700,10 @@
       <c r="H8" s="13">
         <v>1</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>103</v>
-      </c>
+      <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L8" s="13">
         <v>5000</v>
@@ -2733,7 +2719,7 @@
       </c>
       <c r="P8" s="13"/>
       <c r="Q8" s="76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R8" s="77"/>
     </row>
@@ -2741,7 +2727,7 @@
       <c r="B9" s="66"/>
       <c r="C9" s="69"/>
       <c r="D9" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="19">
         <v>2</v>
@@ -2749,12 +2735,10 @@
       <c r="H9" s="13">
         <v>2</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>102</v>
-      </c>
+      <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L9" s="13">
         <v>100000</v>
@@ -2769,10 +2753,10 @@
         <v>100</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q9" s="76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R9" s="77"/>
     </row>
@@ -2780,7 +2764,7 @@
       <c r="B10" s="66"/>
       <c r="C10" s="69"/>
       <c r="D10" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="19">
         <v>3</v>
@@ -2788,12 +2772,10 @@
       <c r="H10" s="13">
         <v>3</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>105</v>
-      </c>
+      <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="13">
         <v>2000</v>
@@ -2808,10 +2790,10 @@
         <v>100</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R10" s="77"/>
     </row>
@@ -2819,7 +2801,7 @@
       <c r="B11" s="66"/>
       <c r="C11" s="69"/>
       <c r="D11" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="19">
         <v>4</v>
@@ -2827,12 +2809,10 @@
       <c r="H11" s="13">
         <v>4</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>113</v>
-      </c>
+      <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L11" s="13">
         <v>1000</v>
@@ -2848,7 +2828,7 @@
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R11" s="77"/>
     </row>
@@ -2856,7 +2836,7 @@
       <c r="B12" s="67"/>
       <c r="C12" s="70"/>
       <c r="D12" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="13"/>
@@ -2876,10 +2856,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="13"/>
@@ -2898,7 +2878,7 @@
       <c r="B14" s="66"/>
       <c r="C14" s="66"/>
       <c r="D14" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="13"/>
@@ -2917,7 +2897,7 @@
       <c r="B15" s="66"/>
       <c r="C15" s="66"/>
       <c r="D15" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="13"/>
@@ -2937,10 +2917,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="68" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="13"/>
@@ -2959,7 +2939,7 @@
       <c r="B17" s="66"/>
       <c r="C17" s="69"/>
       <c r="D17" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="13"/>
@@ -2978,7 +2958,7 @@
       <c r="B18" s="66"/>
       <c r="C18" s="69"/>
       <c r="D18" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="13"/>
@@ -3148,8 +3128,8 @@
   </sheetPr>
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3177,7 +3157,7 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="91"/>
       <c r="D3" s="91"/>
@@ -3194,19 +3174,19 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="89" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="D4" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="E4" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="89" t="s">
-        <v>46</v>
-      </c>
       <c r="F4" s="86" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="87"/>
       <c r="H4" s="87"/>
@@ -3215,7 +3195,7 @@
       <c r="K4" s="87"/>
       <c r="L4" s="88"/>
       <c r="M4" s="85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N4" s="85"/>
     </row>
@@ -3225,29 +3205,29 @@
       <c r="D5" s="99"/>
       <c r="E5" s="90"/>
       <c r="F5" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="73" t="s">
         <v>71</v>
-      </c>
-      <c r="K5" s="73" t="s">
-        <v>72</v>
       </c>
       <c r="L5" s="74"/>
       <c r="M5" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -3255,16 +3235,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>48</v>
-      </c>
       <c r="E6" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="13">
         <v>5000</v>
@@ -3279,16 +3259,16 @@
         <v>1000000</v>
       </c>
       <c r="K6" s="76" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L6" s="77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3298,13 +3278,13 @@
       </c>
       <c r="C7" s="96"/>
       <c r="D7" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="13">
         <v>-2000</v>
@@ -3319,16 +3299,16 @@
         <v>100</v>
       </c>
       <c r="K7" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>78</v>
+      <c r="N7" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3338,13 +3318,13 @@
       </c>
       <c r="C8" s="96"/>
       <c r="D8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="13">
         <v>1000000000</v>
@@ -3359,14 +3339,14 @@
         <v>100</v>
       </c>
       <c r="K8" s="76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L8" s="77"/>
       <c r="M8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="N8" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3376,13 +3356,13 @@
       </c>
       <c r="C9" s="96"/>
       <c r="D9" s="17" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="13">
         <v>1000000000</v>
@@ -3397,14 +3377,14 @@
         <v>100</v>
       </c>
       <c r="K9" s="76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L9" s="77"/>
       <c r="M9" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="N9" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
@@ -3414,13 +3394,13 @@
       </c>
       <c r="C10" s="96"/>
       <c r="D10" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" s="13">
         <v>5000</v>
@@ -3437,10 +3417,10 @@
       <c r="K10" s="83"/>
       <c r="L10" s="84"/>
       <c r="M10" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
@@ -3450,13 +3430,13 @@
       </c>
       <c r="C11" s="96"/>
       <c r="D11" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" s="13">
         <v>100000</v>
@@ -3471,14 +3451,14 @@
         <v>100</v>
       </c>
       <c r="K11" s="83" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L11" s="84"/>
       <c r="M11" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3488,13 +3468,13 @@
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="13">
         <v>2000</v>
@@ -3509,14 +3489,14 @@
         <v>100</v>
       </c>
       <c r="K12" s="83" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L12" s="84"/>
       <c r="M12" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3526,13 +3506,13 @@
       </c>
       <c r="C13" s="97"/>
       <c r="D13" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" s="13">
         <v>1000</v>
@@ -3549,10 +3529,10 @@
       <c r="K13" s="83"/>
       <c r="L13" s="84"/>
       <c r="M13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="N13" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -3572,7 +3552,7 @@
     </row>
     <row r="15" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
@@ -3591,23 +3571,23 @@
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C17" s="92" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
       <c r="F17" s="94"/>
       <c r="G17" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="92" t="s">
         <v>52</v>
-      </c>
-      <c r="H17" s="92" t="s">
-        <v>53</v>
       </c>
       <c r="I17" s="95"/>
       <c r="J17" s="93"/>
       <c r="K17" s="93"/>
       <c r="L17" s="94"/>
       <c r="M17" s="92" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N17" s="95"/>
       <c r="O17" s="93"/>
@@ -3615,47 +3595,47 @@
     </row>
     <row r="18" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="108" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="85" t="s">
+      <c r="E18" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="85" t="s">
+      <c r="F18" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="109" t="s">
+      <c r="G18" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="110" t="s">
+      <c r="H18" s="111" t="s">
         <v>59</v>
-      </c>
-      <c r="H18" s="111" t="s">
-        <v>60</v>
       </c>
       <c r="I18" s="98"/>
       <c r="J18" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="85" t="s">
+      <c r="L18" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="L18" s="109" t="s">
-        <v>57</v>
-      </c>
       <c r="M18" s="100" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N18" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="85" t="s">
+      <c r="P18" s="109" t="s">
         <v>56</v>
-      </c>
-      <c r="P18" s="109" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
@@ -3677,48 +3657,48 @@
     </row>
     <row r="20" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="32">
         <v>8</v>
       </c>
       <c r="D20" s="33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="33">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F20" s="105" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G20" s="105" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H20" s="103"/>
       <c r="I20" s="104"/>
       <c r="J20" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K20" s="33">
         <v>5</v>
       </c>
       <c r="L20" s="34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O20" s="33">
         <v>0</v>
       </c>
       <c r="P20" s="34">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B21" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="32">
         <v>8</v>
@@ -3730,10 +3710,10 @@
         <v>3</v>
       </c>
       <c r="F21" s="105" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G21" s="105" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H21" s="103"/>
       <c r="I21" s="104"/>
@@ -3759,7 +3739,7 @@
     </row>
     <row r="22" spans="2:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B22" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="32">
         <v>8</v>
@@ -3771,10 +3751,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G22" s="105" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H22" s="103"/>
       <c r="I22" s="104"/>

</xml_diff>